<commit_message>
Motor specification excel formatting completed
</commit_message>
<xml_diff>
--- a/thermax_backend/templates/motor_specification_template.xlsx
+++ b/thermax_backend/templates/motor_specification_template.xlsx
@@ -3,18 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAC17D03-D636-45B9-8C74-1D18330A0C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE537D63-837B-46A8-B6F6-5FD3ABFE6B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="919" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="919" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER" sheetId="16" r:id="rId1"/>
     <sheet name="INSTRUCTION PAGE" sheetId="5" r:id="rId2"/>
     <sheet name="SPECIFICATION" sheetId="4" r:id="rId3"/>
-    <sheet name="SAFE AREA MOTOR LIST  " sheetId="11" r:id="rId4"/>
+    <sheet name="SAFE AREA MOTOR LIST" sheetId="11" r:id="rId4"/>
     <sheet name=" SAFE AREA MOTOR BOM" sheetId="12" r:id="rId5"/>
-    <sheet name=" HAZARDOUS AREA MOTOR LIST " sheetId="13" r:id="rId6"/>
-    <sheet name=" HAZARDOUS AREA MOTOR BOM  " sheetId="14" r:id="rId7"/>
+    <sheet name=" HAZARDOUS AREA MOTOR LIST" sheetId="13" r:id="rId6"/>
+    <sheet name=" HAZARDOUS AREA MOTOR BOM" sheetId="14" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">#N/A</definedName>
@@ -39,28 +39,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </valueMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2085,17 +2063,7 @@
     <cellStyle name="Normal 3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2195,71 +2163,51 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1687286</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>145143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3363772</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1307253</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEFCFABC-390D-AFED-E4B8-8F1290487C72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4363357" y="145143"/>
+          <a:ext cx="1676486" cy="1162110"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3174,9 +3122,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="94" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+      <c r="A1" s="94"/>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
       <c r="D1" s="95"/>
@@ -3591,12 +3537,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="98" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A36" zoomScale="98" zoomScaleNormal="100" zoomScaleSheetLayoutView="98" workbookViewId="0">
       <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
@@ -4057,7 +4000,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.25" footer="0.25"/>
-  <pageSetup paperSize="9" scale="98" fitToHeight="100" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="94" fitToHeight="100" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;12Classification: &amp;KFF0000Project Confidential&amp;8&amp;K000000
 </oddHeader>
@@ -4072,7 +4015,7 @@
   </sheetPr>
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A49" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A63" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -4857,10 +4800,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD7"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -5054,124 +4997,23 @@
       <c r="AD3" s="66"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" s="66"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="66"/>
-      <c r="W4" s="66"/>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="66"/>
-      <c r="Z5" s="66"/>
-      <c r="AA5" s="66"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
-      <c r="AD5" s="66"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="66"/>
-      <c r="V6" s="66"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="66"/>
-      <c r="Z6" s="66"/>
-      <c r="AA6" s="66"/>
-      <c r="AB6" s="66"/>
-      <c r="AC6" s="66"/>
-      <c r="AD6" s="66"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="68"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:AD1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1 A7 C7:J7">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:I6 K2:AD6">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1 A2:I3 K2:AD3 A4 C4:J4">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5187,10 +5029,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="115" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F6"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -5242,36 +5084,12 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5280,10 +5098,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD7"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AD6"/>
+    <sheetView view="pageBreakPreview" topLeftCell="Q1" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -5477,124 +5295,23 @@
       <c r="AD3" s="57"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="57"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="57"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="57"/>
-      <c r="W5" s="57"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="57"/>
-      <c r="Z5" s="57"/>
-      <c r="AA5" s="57"/>
-      <c r="AB5" s="57"/>
-      <c r="AC5" s="57"/>
-      <c r="AD5" s="57"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A6" s="57"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="57"/>
-      <c r="W6" s="57"/>
-      <c r="X6" s="57"/>
-      <c r="Y6" s="57"/>
-      <c r="Z6" s="57"/>
-      <c r="AA6" s="57"/>
-      <c r="AB6" s="57"/>
-      <c r="AC6" s="57"/>
-      <c r="AD6" s="57"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:AD1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1 A7 C7:J7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:I6 K2:AD6">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1 A2:I3 K2:AD3 A4 C4:J4">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5610,17 +5327,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F6"/>
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="49.54296875" style="74" customWidth="1"/>
+    <col min="3" max="3" width="75.08984375" style="74" customWidth="1"/>
     <col min="4" max="4" width="5.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7265625" style="3" customWidth="1"/>
@@ -5665,36 +5382,12 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>